<commit_message>
executed simulations (research study)
</commit_message>
<xml_diff>
--- a/simulation_reports/normal_load/normal_load.xlsx
+++ b/simulation_reports/normal_load/normal_load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/simulation_reports/normal_load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A1AD6E-19D8-0045-8033-601D2E9BF771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642226FE-280F-8A47-A758-E1A726C1AD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{E6A8C358-B2E9-494F-8740-18BB613A17CD}"/>
+    <workbookView xWindow="460" yWindow="780" windowWidth="28040" windowHeight="16320" xr2:uid="{E6A8C358-B2E9-494F-8740-18BB613A17CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5233,7 +5229,7 @@
   <dimension ref="A1:B656"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>